<commit_message>
ádám se marad ki a buliból
</commit_message>
<xml_diff>
--- a/BeadandóKövetelményStatikusWeboldal.xlsx
+++ b/BeadandóKövetelményStatikusWeboldal.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gamer\Desktop\weboldalak\fukkosalegnagyobbkiraly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\WebProg\Projektmunka\fukkosalegnagyobbkiraly\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33469DE-039D-4E5D-A9C9-3A8B557379FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27630" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fedőlap" sheetId="2" r:id="rId1"/>
@@ -20,20 +21,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Irányelvek!$A$1:$L$42</definedName>
     <definedName name="nem_modosithato2">Irányelvek!$J:$J,Irányelvek!$I:$I,Irányelvek!$H$1,Irányelvek!$G:$G,Irányelvek!$H:$H,Irányelvek!$F:$F,Irányelvek!$C:$C,Irányelvek!$B:$B,Irányelvek!$A:$A</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -322,20 +310,20 @@
     </r>
   </si>
   <si>
-    <t>Dobrovenszki Balázs</t>
+    <t>dobrovenszkibalazs@ckik.hu</t>
   </si>
   <si>
-    <t>dobrovenszkibalazs@ckik.hu</t>
+    <t>Dobrovenszki Balázs, Varga Ádám</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _F_t_-;\-* #,##0.00\ _F_t_-;_-* &quot;-&quot;??\ _F_t_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode=";;;"/>
-    <numFmt numFmtId="165" formatCode="#,##0_ ;\-#,##0\ "/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _F_t_-;\-* #,##0.00\ _F_t_-;_-* &quot;-&quot;??\ _F_t_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode=";;;"/>
+    <numFmt numFmtId="166" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
@@ -736,7 +724,7 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
@@ -752,12 +740,12 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -775,48 +763,48 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -885,14 +873,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -8516,9 +8504,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -8556,9 +8544,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -8593,7 +8581,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -8628,7 +8616,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -8801,12 +8789,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Munka1"/>
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8825,15 +8813,15 @@
   <sheetData>
     <row r="1" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="52"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
       <c r="I1" s="52"/>
       <c r="J1" s="52"/>
     </row>
@@ -8843,7 +8831,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="62" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D2" s="63"/>
       <c r="E2" s="63"/>
@@ -8859,7 +8847,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="64" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D3" s="63"/>
       <c r="E3" s="63"/>
@@ -8938,10 +8926,10 @@
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="52"/>
-      <c r="B9" s="60" t="s">
+      <c r="B9" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="60"/>
+      <c r="C9" s="58"/>
       <c r="D9" s="51">
         <f>COUNTA(Irányelvek!C:C)-1</f>
         <v>41</v>
@@ -8957,10 +8945,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="52"/>
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="60"/>
+      <c r="C10" s="58"/>
       <c r="D10" s="51">
         <f>SUM(Irányelvek!G:G)</f>
         <v>70</v>
@@ -8974,10 +8962,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="52"/>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="60"/>
+      <c r="C11" s="58"/>
       <c r="D11" s="51">
         <v>30</v>
       </c>
@@ -8990,10 +8978,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="52"/>
-      <c r="B12" s="60" t="s">
+      <c r="B12" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="60"/>
+      <c r="C12" s="58"/>
       <c r="D12" s="51">
         <v>10</v>
       </c>
@@ -9006,10 +8994,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="52"/>
-      <c r="B13" s="60" t="s">
+      <c r="B13" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="60"/>
+      <c r="C13" s="58"/>
       <c r="D13" s="51">
         <v>30</v>
       </c>
@@ -9036,10 +9024,10 @@
     </row>
     <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="52"/>
-      <c r="B15" s="60" t="s">
+      <c r="B15" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="60"/>
+      <c r="C15" s="58"/>
       <c r="D15" s="51" t="b">
         <f t="array" ref="D15">IF(COUNTIFS(Irányelvek!D2:D42,"=hamis",Irányelvek!F2:F42,"=Igaz")=0,TRUE,FALSE)</f>
         <v>0</v>
@@ -9053,10 +9041,10 @@
     </row>
     <row r="16" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="52"/>
-      <c r="B16" s="60" t="s">
+      <c r="B16" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="60"/>
+      <c r="C16" s="58"/>
       <c r="D16" s="54">
         <f>SUM(Irányelvek!H2:H42)</f>
         <v>63</v>
@@ -9090,10 +9078,10 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="52"/>
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="60"/>
+      <c r="C18" s="58"/>
       <c r="D18" s="57"/>
       <c r="E18" s="52"/>
       <c r="F18" s="70"/>
@@ -9104,10 +9092,10 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="52"/>
-      <c r="B19" s="60" t="s">
+      <c r="B19" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="60"/>
+      <c r="C19" s="58"/>
       <c r="D19" s="54">
         <f>SUM(D16:D18)</f>
         <v>63</v>
@@ -9137,6 +9125,8 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="GY0qzS23AjeU4FiVxM6V6yTeqAyuwIwkf0prt1k9kjvXMb2kI4aIbHicosNGGfE24sgSmE5PyGQO+AcVTCjtsg==" saltValue="Ta2LPohq4QT75tLdf5jIUQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="18">
+    <mergeCell ref="F16:H18"/>
+    <mergeCell ref="F9:H13"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B1:H1"/>
@@ -9153,8 +9143,6 @@
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="F16:H18"/>
-    <mergeCell ref="F9:H13"/>
   </mergeCells>
   <conditionalFormatting sqref="D16:D19">
     <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
@@ -9162,8 +9150,8 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="B5" location="Irányelvek!A1" display="Az irányelvek megtekintése és az adatlap kitöltése"/>
-    <hyperlink ref="B5:H5" location="Irányelvek!A1" display="Az irányelvek megtekintése és az adatlap kitöltése"/>
+    <hyperlink ref="B5" location="Irányelvek!A1" display="Az irányelvek megtekintése és az adatlap kitöltése" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B5:H5" location="Irányelvek!A1" display="Az irányelvek megtekintése és az adatlap kitöltése" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -9171,7 +9159,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Munka2"/>
   <dimension ref="A1:L42"/>
   <sheetViews>
@@ -12447,12 +12435,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Munka6"/>
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>